<commit_message>
Corrige o cálculo do MtM multiplicando as taxas da B3 por 100.
</commit_message>
<xml_diff>
--- a/validacao_mtm.xlsx
+++ b/validacao_mtm.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J21"/>
+  <dimension ref="A1:J12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -491,41 +491,41 @@
     </row>
     <row r="2">
       <c r="A2" t="n">
-        <v>9</v>
+        <v>1</v>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>DI1F29</t>
+          <t>DI1F27</t>
         </is>
       </c>
       <c r="C2" s="2" t="n">
         <v>45846</v>
       </c>
       <c r="D2" t="n">
-        <v>13.31</v>
+        <v>14.21</v>
       </c>
       <c r="E2" t="n">
-        <v>0.1331</v>
+        <v>14.18</v>
       </c>
       <c r="F2" s="2" t="n">
         <v>45845</v>
       </c>
       <c r="G2" t="n">
-        <v>13.31</v>
+        <v>14.2</v>
       </c>
       <c r="H2" t="n">
-        <v>0.1331</v>
+        <v>14.2</v>
       </c>
       <c r="I2" t="n">
-        <v>17.93412781335064</v>
+        <v>63.307401682614</v>
       </c>
       <c r="J2" t="n">
-        <v>0</v>
+        <v>-0.09999999999998899</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="n">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="B3" t="inlineStr">
         <is>
@@ -533,33 +533,31 @@
         </is>
       </c>
       <c r="C3" s="2" t="n">
-        <v>45846</v>
+        <v>45845</v>
       </c>
       <c r="D3" t="n">
         <v>13.31</v>
       </c>
       <c r="E3" t="n">
-        <v>0.1331</v>
+        <v>13.31</v>
       </c>
       <c r="F3" s="2" t="n">
-        <v>45845</v>
+        <v>45842</v>
       </c>
       <c r="G3" t="n">
-        <v>13.31</v>
-      </c>
-      <c r="H3" t="n">
-        <v>0.1331</v>
-      </c>
+        <v>13.21</v>
+      </c>
+      <c r="H3" t="inlineStr"/>
       <c r="I3" t="n">
-        <v>-71.73651125340257</v>
+        <v>1013.273002577334</v>
       </c>
       <c r="J3" t="n">
-        <v>0</v>
+        <v>0.4999999999999893</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="n">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="B4" t="inlineStr">
         <is>
@@ -567,33 +565,31 @@
         </is>
       </c>
       <c r="C4" s="2" t="n">
-        <v>45846</v>
+        <v>45845</v>
       </c>
       <c r="D4" t="n">
         <v>13.31</v>
       </c>
       <c r="E4" t="n">
-        <v>0.1331</v>
+        <v>13.31</v>
       </c>
       <c r="F4" s="2" t="n">
-        <v>45845</v>
+        <v>45842</v>
       </c>
       <c r="G4" t="n">
-        <v>13.31</v>
-      </c>
-      <c r="H4" t="n">
-        <v>0.1331</v>
-      </c>
+        <v>13.21</v>
+      </c>
+      <c r="H4" t="inlineStr"/>
       <c r="I4" t="n">
-        <v>71.73651125340257</v>
+        <v>-4053.092010309338</v>
       </c>
       <c r="J4" t="n">
-        <v>0</v>
+        <v>1.999999999999957</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="n">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B5" t="inlineStr">
         <is>
@@ -601,135 +597,127 @@
         </is>
       </c>
       <c r="C5" s="2" t="n">
-        <v>45846</v>
+        <v>45845</v>
       </c>
       <c r="D5" t="n">
         <v>13.31</v>
       </c>
       <c r="E5" t="n">
-        <v>0.1331</v>
+        <v>13.31</v>
       </c>
       <c r="F5" s="2" t="n">
-        <v>45845</v>
+        <v>45842</v>
       </c>
       <c r="G5" t="n">
-        <v>13.31</v>
-      </c>
-      <c r="H5" t="n">
-        <v>0.1331</v>
-      </c>
+        <v>13.21</v>
+      </c>
+      <c r="H5" t="inlineStr"/>
       <c r="I5" t="n">
-        <v>-17.93412781335064</v>
+        <v>4053.092010309338</v>
       </c>
       <c r="J5" t="n">
-        <v>0</v>
+        <v>1.999999999999957</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="n">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>DI1F31</t>
+          <t>DI1F29</t>
         </is>
       </c>
       <c r="C6" s="2" t="n">
-        <v>45846</v>
+        <v>45845</v>
       </c>
       <c r="D6" t="n">
-        <v>13.42</v>
+        <v>13.31</v>
       </c>
       <c r="E6" t="n">
-        <v>0.1342</v>
+        <v>13.31</v>
       </c>
       <c r="F6" s="2" t="n">
-        <v>45845</v>
+        <v>45842</v>
       </c>
       <c r="G6" t="n">
-        <v>13.4</v>
-      </c>
-      <c r="H6" t="n">
-        <v>0.134</v>
-      </c>
+        <v>13.21</v>
+      </c>
+      <c r="H6" t="inlineStr"/>
       <c r="I6" t="n">
-        <v>-510.4255816614022</v>
+        <v>-1013.273002577334</v>
       </c>
       <c r="J6" t="n">
-        <v>0.00199999999999978</v>
+        <v>0.4999999999999893</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="n">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>DI1F27</t>
+          <t>DI1F31</t>
         </is>
       </c>
       <c r="C7" s="2" t="n">
-        <v>45846</v>
+        <v>45845</v>
       </c>
       <c r="D7" t="n">
-        <v>14.21</v>
+        <v>13.4</v>
       </c>
       <c r="E7" t="n">
-        <v>0.1418</v>
+        <v>13.4</v>
       </c>
       <c r="F7" s="2" t="n">
-        <v>45845</v>
+        <v>45842</v>
       </c>
       <c r="G7" t="n">
-        <v>14.2</v>
-      </c>
-      <c r="H7" t="n">
-        <v>0.142</v>
-      </c>
+        <v>13.27</v>
+      </c>
+      <c r="H7" t="inlineStr"/>
       <c r="I7" t="n">
-        <v>63.307401682614</v>
+        <v>-3189.938378095758</v>
       </c>
       <c r="J7" t="n">
-        <v>-0.0009999999999998899</v>
+        <v>1.300000000000008</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="n">
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>DI1F26</t>
+          <t>DI1F27</t>
         </is>
       </c>
       <c r="C8" s="2" t="n">
-        <v>45846</v>
+        <v>45845</v>
       </c>
       <c r="D8" t="n">
-        <v>14.92</v>
+        <v>14.2</v>
       </c>
       <c r="E8" t="n">
-        <v>0.1492</v>
+        <v>14.2</v>
       </c>
       <c r="F8" s="2" t="n">
-        <v>45845</v>
+        <v>45842</v>
       </c>
       <c r="G8" t="n">
-        <v>14.92</v>
-      </c>
-      <c r="H8" t="n">
-        <v>0.1492</v>
-      </c>
+        <v>14.16</v>
+      </c>
+      <c r="H8" t="inlineStr"/>
       <c r="I8" t="n">
-        <v>-0.966951289519784</v>
+        <v>224.5059976513585</v>
       </c>
       <c r="J8" t="n">
-        <v>0</v>
+        <v>0.1999999999999957</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="n">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="B9" t="inlineStr">
         <is>
@@ -737,67 +725,63 @@
         </is>
       </c>
       <c r="C9" s="2" t="n">
-        <v>45846</v>
+        <v>45845</v>
       </c>
       <c r="D9" t="n">
         <v>14.92</v>
       </c>
       <c r="E9" t="n">
-        <v>0.1492</v>
+        <v>14.92</v>
       </c>
       <c r="F9" s="2" t="n">
-        <v>45845</v>
+        <v>45842</v>
       </c>
       <c r="G9" t="n">
-        <v>14.92</v>
-      </c>
-      <c r="H9" t="n">
-        <v>0.1492</v>
-      </c>
+        <v>14.91</v>
+      </c>
+      <c r="H9" t="inlineStr"/>
       <c r="I9" t="n">
-        <v>1.933902579039568</v>
+        <v>60.39976826075872</v>
       </c>
       <c r="J9" t="n">
-        <v>0</v>
+        <v>0.1499999999999968</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="n">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>DI1N26</t>
+          <t>DI1F26</t>
         </is>
       </c>
       <c r="C10" s="2" t="n">
-        <v>45846</v>
+        <v>45845</v>
       </c>
       <c r="D10" t="n">
-        <v>14.7</v>
+        <v>14.92</v>
       </c>
       <c r="E10" t="n">
-        <v>0.147</v>
+        <v>14.92</v>
       </c>
       <c r="F10" s="2" t="n">
-        <v>45845</v>
+        <v>45842</v>
       </c>
       <c r="G10" t="n">
-        <v>14.71</v>
-      </c>
-      <c r="H10" t="n">
-        <v>0.1471</v>
-      </c>
+        <v>14.91</v>
+      </c>
+      <c r="H10" t="inlineStr"/>
       <c r="I10" t="n">
-        <v>137.9160259410855</v>
+        <v>-120.7995365215174</v>
       </c>
       <c r="J10" t="n">
-        <v>-0.002000000000000335</v>
+        <v>0.2999999999999936</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B11" t="inlineStr">
         <is>
@@ -805,368 +789,58 @@
         </is>
       </c>
       <c r="C11" s="2" t="n">
-        <v>45846</v>
+        <v>45845</v>
       </c>
       <c r="D11" t="n">
-        <v>14.7</v>
+        <v>14.71</v>
       </c>
       <c r="E11" t="n">
-        <v>0.147</v>
+        <v>14.71</v>
       </c>
       <c r="F11" s="2" t="n">
-        <v>45845</v>
+        <v>45842</v>
       </c>
       <c r="G11" t="n">
-        <v>14.71</v>
-      </c>
-      <c r="H11" t="n">
-        <v>0.1471</v>
-      </c>
+        <v>14.68</v>
+      </c>
+      <c r="H11" t="inlineStr"/>
       <c r="I11" t="n">
-        <v>-137.9160259410855</v>
+        <v>-463.1330171364243</v>
       </c>
       <c r="J11" t="n">
-        <v>-0.002000000000000335</v>
+        <v>0.6000000000000227</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="n">
-        <v>9</v>
+        <v>2</v>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>DI1F29</t>
+          <t>DI1N26</t>
         </is>
       </c>
       <c r="C12" s="2" t="n">
         <v>45845</v>
       </c>
       <c r="D12" t="n">
-        <v>13.31</v>
+        <v>14.71</v>
       </c>
       <c r="E12" t="n">
-        <v>0.1331</v>
+        <v>14.71</v>
       </c>
       <c r="F12" s="2" t="n">
         <v>45842</v>
       </c>
       <c r="G12" t="n">
-        <v>13.21</v>
-      </c>
-      <c r="H12" t="n">
-        <v>0.1323</v>
-      </c>
+        <v>14.68</v>
+      </c>
+      <c r="H12" t="inlineStr"/>
       <c r="I12" t="n">
-        <v>1013.273002577334</v>
+        <v>463.1330171364243</v>
       </c>
       <c r="J12" t="n">
-        <v>0.003999999999999976</v>
-      </c>
-    </row>
-    <row r="13">
-      <c r="A13" t="n">
-        <v>4</v>
-      </c>
-      <c r="B13" t="inlineStr">
-        <is>
-          <t>DI1F29</t>
-        </is>
-      </c>
-      <c r="C13" s="2" t="n">
-        <v>45845</v>
-      </c>
-      <c r="D13" t="n">
-        <v>13.31</v>
-      </c>
-      <c r="E13" t="n">
-        <v>0.1331</v>
-      </c>
-      <c r="F13" s="2" t="n">
-        <v>45842</v>
-      </c>
-      <c r="G13" t="n">
-        <v>13.21</v>
-      </c>
-      <c r="H13" t="n">
-        <v>0.1323</v>
-      </c>
-      <c r="I13" t="n">
-        <v>-4053.092010309338</v>
-      </c>
-      <c r="J13" t="n">
-        <v>0.0159999999999999</v>
-      </c>
-    </row>
-    <row r="14">
-      <c r="A14" t="n">
-        <v>8</v>
-      </c>
-      <c r="B14" t="inlineStr">
-        <is>
-          <t>DI1F29</t>
-        </is>
-      </c>
-      <c r="C14" s="2" t="n">
-        <v>45845</v>
-      </c>
-      <c r="D14" t="n">
-        <v>13.31</v>
-      </c>
-      <c r="E14" t="n">
-        <v>0.1331</v>
-      </c>
-      <c r="F14" s="2" t="n">
-        <v>45842</v>
-      </c>
-      <c r="G14" t="n">
-        <v>13.21</v>
-      </c>
-      <c r="H14" t="n">
-        <v>0.1323</v>
-      </c>
-      <c r="I14" t="n">
-        <v>4053.092010309338</v>
-      </c>
-      <c r="J14" t="n">
-        <v>0.0159999999999999</v>
-      </c>
-    </row>
-    <row r="15">
-      <c r="A15" t="n">
-        <v>7</v>
-      </c>
-      <c r="B15" t="inlineStr">
-        <is>
-          <t>DI1F29</t>
-        </is>
-      </c>
-      <c r="C15" s="2" t="n">
-        <v>45845</v>
-      </c>
-      <c r="D15" t="n">
-        <v>13.31</v>
-      </c>
-      <c r="E15" t="n">
-        <v>0.1331</v>
-      </c>
-      <c r="F15" s="2" t="n">
-        <v>45842</v>
-      </c>
-      <c r="G15" t="n">
-        <v>13.21</v>
-      </c>
-      <c r="H15" t="n">
-        <v>0.1323</v>
-      </c>
-      <c r="I15" t="n">
-        <v>-1013.273002577334</v>
-      </c>
-      <c r="J15" t="n">
-        <v>0.003999999999999976</v>
-      </c>
-    </row>
-    <row r="16">
-      <c r="A16" t="n">
-        <v>6</v>
-      </c>
-      <c r="B16" t="inlineStr">
-        <is>
-          <t>DI1F31</t>
-        </is>
-      </c>
-      <c r="C16" s="2" t="n">
-        <v>45845</v>
-      </c>
-      <c r="D16" t="n">
-        <v>13.4</v>
-      </c>
-      <c r="E16" t="n">
-        <v>0.134</v>
-      </c>
-      <c r="F16" s="2" t="n">
-        <v>45842</v>
-      </c>
-      <c r="G16" t="n">
-        <v>13.27</v>
-      </c>
-      <c r="H16" t="n">
-        <v>0.133</v>
-      </c>
-      <c r="I16" t="n">
-        <v>-3189.938378095758</v>
-      </c>
-      <c r="J16" t="n">
-        <v>0.01000000000000001</v>
-      </c>
-    </row>
-    <row r="17">
-      <c r="A17" t="n">
-        <v>1</v>
-      </c>
-      <c r="B17" t="inlineStr">
-        <is>
-          <t>DI1F27</t>
-        </is>
-      </c>
-      <c r="C17" s="2" t="n">
-        <v>45845</v>
-      </c>
-      <c r="D17" t="n">
-        <v>14.2</v>
-      </c>
-      <c r="E17" t="n">
-        <v>0.142</v>
-      </c>
-      <c r="F17" s="2" t="n">
-        <v>45842</v>
-      </c>
-      <c r="G17" t="n">
-        <v>14.16</v>
-      </c>
-      <c r="H17" t="n">
-        <v>0.1418</v>
-      </c>
-      <c r="I17" t="n">
-        <v>224.5059976513585</v>
-      </c>
-      <c r="J17" t="n">
-        <v>0.0009999999999998899</v>
-      </c>
-    </row>
-    <row r="18">
-      <c r="A18" t="n">
-        <v>10</v>
-      </c>
-      <c r="B18" t="inlineStr">
-        <is>
-          <t>DI1F26</t>
-        </is>
-      </c>
-      <c r="C18" s="2" t="n">
-        <v>45845</v>
-      </c>
-      <c r="D18" t="n">
-        <v>14.92</v>
-      </c>
-      <c r="E18" t="n">
-        <v>0.1492</v>
-      </c>
-      <c r="F18" s="2" t="n">
-        <v>45842</v>
-      </c>
-      <c r="G18" t="n">
-        <v>14.91</v>
-      </c>
-      <c r="H18" t="n">
-        <v>0.1492</v>
-      </c>
-      <c r="I18" t="n">
-        <v>60.39976826075872</v>
-      </c>
-      <c r="J18" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="19">
-      <c r="A19" t="n">
-        <v>5</v>
-      </c>
-      <c r="B19" t="inlineStr">
-        <is>
-          <t>DI1F26</t>
-        </is>
-      </c>
-      <c r="C19" s="2" t="n">
-        <v>45845</v>
-      </c>
-      <c r="D19" t="n">
-        <v>14.92</v>
-      </c>
-      <c r="E19" t="n">
-        <v>0.1492</v>
-      </c>
-      <c r="F19" s="2" t="n">
-        <v>45842</v>
-      </c>
-      <c r="G19" t="n">
-        <v>14.91</v>
-      </c>
-      <c r="H19" t="n">
-        <v>0.1492</v>
-      </c>
-      <c r="I19" t="n">
-        <v>-120.7995365215174</v>
-      </c>
-      <c r="J19" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="20">
-      <c r="A20" t="n">
-        <v>3</v>
-      </c>
-      <c r="B20" t="inlineStr">
-        <is>
-          <t>DI1N26</t>
-        </is>
-      </c>
-      <c r="C20" s="2" t="n">
-        <v>45845</v>
-      </c>
-      <c r="D20" t="n">
-        <v>14.71</v>
-      </c>
-      <c r="E20" t="n">
-        <v>0.1471</v>
-      </c>
-      <c r="F20" s="2" t="n">
-        <v>45842</v>
-      </c>
-      <c r="G20" t="n">
-        <v>14.68</v>
-      </c>
-      <c r="H20" t="n">
-        <v>0.1469</v>
-      </c>
-      <c r="I20" t="n">
-        <v>-463.1330171364243</v>
-      </c>
-      <c r="J20" t="n">
-        <v>0.004000000000000115</v>
-      </c>
-    </row>
-    <row r="21">
-      <c r="A21" t="n">
-        <v>2</v>
-      </c>
-      <c r="B21" t="inlineStr">
-        <is>
-          <t>DI1N26</t>
-        </is>
-      </c>
-      <c r="C21" s="2" t="n">
-        <v>45845</v>
-      </c>
-      <c r="D21" t="n">
-        <v>14.71</v>
-      </c>
-      <c r="E21" t="n">
-        <v>0.1471</v>
-      </c>
-      <c r="F21" s="2" t="n">
-        <v>45842</v>
-      </c>
-      <c r="G21" t="n">
-        <v>14.68</v>
-      </c>
-      <c r="H21" t="n">
-        <v>0.1469</v>
-      </c>
-      <c r="I21" t="n">
-        <v>463.1330171364243</v>
-      </c>
-      <c r="J21" t="n">
-        <v>0.004000000000000115</v>
+        <v>0.6000000000000227</v>
       </c>
     </row>
   </sheetData>

</xml_diff>